<commit_message>
SEX_AGE_DATA file updated and renamed as gender_age
</commit_message>
<xml_diff>
--- a/gender_age_metadata.xlsx
+++ b/gender_age_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dunleavyjason/Documents/Metis/project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{70490D51-8C3D-444A-8978-AF38FF111410}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CF3CE05B-16B7-1846-B27E-23B220FFE2B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260"/>
   </bookViews>
@@ -2970,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B358"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Jason's updates Jan 5 PM
</commit_message>
<xml_diff>
--- a/gender_age_metadata.xlsx
+++ b/gender_age_metadata.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dunleavyjason/Documents/Metis/project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CF3CE05B-16B7-1846-B27E-23B220FFE2B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A790718F-8856-074E-B72D-71DC5BDD8009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260"/>
+    <workbookView xWindow="-2540" yWindow="-24640" windowWidth="34880" windowHeight="22780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gender_age_metadata" sheetId="1" r:id="rId1"/>
@@ -2125,7 +2125,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2967,11 +2967,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3828,10 +3828,10 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="1" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3860,10 +3860,10 @@
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="1" t="s">
         <v>217</v>
       </c>
     </row>

</xml_diff>